<commit_message>
Journal et planning mis à jour
</commit_message>
<xml_diff>
--- a/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
+++ b/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\harmony\v2_06\apps\2309_AutomatisationPriseImageRTI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BE3E1C-D230-4498-A473-46F540278A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFEB076-F7D5-4369-9FDF-6DAADD2A2BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -74,7 +74,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Reception cahier des charges, mise en place des documents de base</t>
+    <t>Nbr de café</t>
+  </si>
+  <si>
+    <t>Reception cahier des charges, mise en place des documents de base, recherche d'information par rapport à la puissance du moteur</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,18 +195,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +481,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E41"/>
+  <dimension ref="B2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,10 +493,11 @@
     <col min="2" max="2" width="10.73046875" style="1"/>
     <col min="3" max="3" width="11.265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="154.73046875" customWidth="1"/>
+    <col min="5" max="5" width="144.59765625" customWidth="1"/>
+    <col min="6" max="6" width="16.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
@@ -515,8 +510,11 @@
       <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -525,10 +523,13 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -537,8 +538,9 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -547,8 +549,9 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -557,8 +560,9 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -567,8 +571,9 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -577,8 +582,9 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,8 +593,9 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -597,8 +604,9 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
@@ -607,8 +615,9 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
@@ -617,8 +626,9 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
@@ -627,8 +637,9 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
@@ -637,8 +648,9 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
@@ -647,8 +659,9 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
@@ -657,8 +670,9 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -667,8 +681,9 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -677,8 +692,9 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
@@ -687,8 +703,9 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -697,8 +714,9 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
@@ -707,8 +725,9 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
@@ -717,8 +736,9 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
@@ -727,8 +747,9 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
@@ -737,8 +758,9 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="6" t="s">
         <v>9</v>
       </c>
@@ -747,8 +769,9 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="6" t="s">
         <v>4</v>
       </c>
@@ -757,8 +780,9 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
@@ -767,8 +791,9 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="6" t="s">
         <v>10</v>
       </c>
@@ -777,8 +802,9 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="6" t="s">
         <v>6</v>
       </c>
@@ -787,8 +813,9 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
@@ -797,8 +824,9 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
@@ -807,8 +835,9 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
@@ -817,8 +846,9 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
@@ -827,8 +857,9 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
@@ -837,8 +868,9 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
         <v>10</v>
       </c>
@@ -847,8 +879,9 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
@@ -857,8 +890,9 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
@@ -867,8 +901,9 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B38" s="6" t="s">
         <v>7</v>
       </c>
@@ -877,14 +912,12 @@
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="12"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C40" s="6" t="s">
         <v>11</v>
       </c>
@@ -892,12 +925,10 @@
         <f>SUM(D3:D39)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
+      <c r="F40">
+        <f>SUM(F3:F38)</f>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Journal et planning updated
</commit_message>
<xml_diff>
--- a/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
+++ b/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\harmony\v2_06\apps\2309_AutomatisationPriseImageRTI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFEB076-F7D5-4369-9FDF-6DAADD2A2BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52D608-1FF0-4AFE-840D-C73807361794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -77,7 +77,10 @@
     <t>Nbr de café</t>
   </si>
   <si>
-    <t>Reception cahier des charges, mise en place des documents de base, recherche d'information par rapport à la puissance du moteur</t>
+    <t>Reception et analyse du cahier des charges, mise en place des documents de base, recherche d'informations par rapport à la puissance du moteur et des LEDs</t>
+  </si>
+  <si>
+    <t>Correction du planning, recherche d'informations et de composants pour le driver de moteur pas à pas, meeting d'une heure</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="B2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -521,7 +524,9 @@
       <c r="C3" s="3">
         <v>45145</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
@@ -536,9 +541,15 @@
       <c r="C4" s="3">
         <v>45146</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
@@ -923,11 +934,11 @@
       </c>
       <c r="D40" s="6">
         <f>SUM(D3:D39)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F40">
         <f>SUM(F3:F38)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PWM for stepper motor fixed at 75%
</commit_message>
<xml_diff>
--- a/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
+++ b/doc/2309_AutomatisationPriseImageRTI-JOURNAL_v1.0.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\harmony\v2_06\apps\2309_AutomatisationPriseImageRTI\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C989755B-3C3A-45F7-89B4-6903F0EDDCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E572A4E-191E-4025-85DD-F5EFAAA0F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Envoi du boitier à imprimer, test des optocoupleurs, test du contact Reed, programmation de l'affichage et des menus</t>
+  </si>
+  <si>
+    <t>Programmation des menus et correction</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="B2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -957,9 +960,15 @@
       <c r="C27" s="7">
         <v>45169</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="D27" s="6">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="9">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="6" t="s">
@@ -1091,11 +1100,11 @@
       </c>
       <c r="D40" s="6">
         <f>SUM(D3:D39)</f>
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F40">
         <f>SUM(F3:F38)</f>
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>